<commit_message>
aws rds insert test completed
</commit_message>
<xml_diff>
--- a/data/news/2022-03-21_news.xlsx
+++ b/data/news/2022-03-21_news.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\news_analysis\data\news\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC4B255-4F42-4BD9-9BE4-156E1FC7BF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC72E1FB-E5BD-41F5-8611-B3D5F6A8A793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59865" yWindow="2400" windowWidth="18720" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="62205" yWindow="2880" windowWidth="18720" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4212,9 +4212,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>new_topic</t>
-  </si>
-  <si>
     <t>news_title</t>
   </si>
   <si>
@@ -4225,6 +4222,10 @@
   </si>
   <si>
     <t>news_text</t>
+  </si>
+  <si>
+    <t>news_topic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4599,7 +4600,7 @@
   <dimension ref="A1:I215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -4619,19 +4620,19 @@
         <v>796</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>798</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>800</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">

</xml_diff>